<commit_message>
Edited font of ALS - Bug Report.xlsx
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS - Bug Report.xlsx
+++ b/documentation/quality/ALS - Bug Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer2\Documents\Not Mine - KIMMY\QUALITY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV-IT111\apc-softdev-it111-05\documentation\quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,36 +100,38 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -230,53 +232,53 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,185 +561,185 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36" style="8" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="18.140625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="36" style="4" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>42016</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>42106</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -746,119 +748,123 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="13" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>1</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
         <v>2</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
         <v>3</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
         <v>4</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>5</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
         <v>6</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
         <v>7</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>8</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>9</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
         <v>10</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
@@ -868,11 +874,8 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>